<commit_message>
fix typo of indexes
</commit_message>
<xml_diff>
--- a/With Information/ParallelHomogeneousWithInfomationProvider.xlsx
+++ b/With Information/ParallelHomogeneousWithInfomationProvider.xlsx
@@ -13,7 +13,187 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>c_p</t>
+  </si>
+  <si>
+    <t>c_i</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>B_org</t>
+  </si>
+  <si>
+    <t>fval</t>
+  </si>
+  <si>
+    <t>flag_q</t>
+  </si>
+  <si>
+    <t>flag_p</t>
+  </si>
+  <si>
+    <t>flag_T</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>c_p</t>
+  </si>
+  <si>
+    <t>c_i</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>B_org</t>
+  </si>
+  <si>
+    <t>fval</t>
+  </si>
+  <si>
+    <t>flag_q</t>
+  </si>
+  <si>
+    <t>flag_p</t>
+  </si>
+  <si>
+    <t>flag_T</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>c_p</t>
+  </si>
+  <si>
+    <t>c_i</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>B_org</t>
+  </si>
+  <si>
+    <t>fval</t>
+  </si>
+  <si>
+    <t>flag_q</t>
+  </si>
+  <si>
+    <t>flag_p</t>
+  </si>
+  <si>
+    <t>flag_T</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>c_p</t>
+  </si>
+  <si>
+    <t>c_i</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>B_org</t>
+  </si>
+  <si>
+    <t>fval</t>
+  </si>
+  <si>
+    <t>flag_q</t>
+  </si>
+  <si>
+    <t>flag_p</t>
+  </si>
+  <si>
+    <t>flag_T</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>c_p</t>
+  </si>
+  <si>
+    <t>c_i</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>B_org</t>
+  </si>
+  <si>
+    <t>fval</t>
+  </si>
+  <si>
+    <t>flag_q</t>
+  </si>
+  <si>
+    <t>flag_p</t>
+  </si>
+  <si>
+    <t>flag_T</t>
+  </si>
   <si>
     <t>M</t>
   </si>
@@ -141,7 +321,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -152,15 +332,25 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -189,40 +379,40 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2">
@@ -239,13 +429,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="0">
-        <v>0.70969875152257245</v>
+        <v>0.72155591310289047</v>
       </c>
       <c r="F2" s="0">
         <v>1</v>
       </c>
       <c r="G2" s="0">
-        <v>0.51543511572225842</v>
+        <v>0.51783640594870639</v>
       </c>
       <c r="H2" s="0">
         <v>0.75</v>
@@ -275,13 +465,13 @@
         <v>0.10000000000000001</v>
       </c>
       <c r="E3" s="0">
-        <v>0.71923207179474824</v>
+        <v>0.73033464779552981</v>
       </c>
       <c r="F3" s="0">
         <v>1</v>
       </c>
       <c r="G3" s="0">
-        <v>0.48026529525957545</v>
+        <v>0.48226681424374995</v>
       </c>
       <c r="H3" s="0">
         <v>0.75</v>
@@ -311,13 +501,13 @@
         <v>0.20000000000000001</v>
       </c>
       <c r="E4" s="0">
-        <v>0.73093785823913981</v>
+        <v>0.73890647070283499</v>
       </c>
       <c r="F4" s="0">
         <v>1</v>
       </c>
       <c r="G4" s="0">
-        <v>0.45619525197236654</v>
+        <v>0.4570670737329014</v>
       </c>
       <c r="H4" s="0">
         <v>0.75</v>
@@ -347,13 +537,13 @@
         <v>0.29999999999999999</v>
       </c>
       <c r="E5" s="0">
-        <v>0.7290342611473456</v>
+        <v>0.74171435119128082</v>
       </c>
       <c r="F5" s="0">
         <v>1</v>
       </c>
       <c r="G5" s="0">
-        <v>0.43518684875791408</v>
+        <v>0.43817092763914656</v>
       </c>
       <c r="H5" s="0">
         <v>0.75</v>
@@ -383,13 +573,13 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="E6" s="0">
-        <v>0.73841563919408038</v>
+        <v>0.7493388853304237</v>
       </c>
       <c r="F6" s="0">
         <v>1</v>
       </c>
       <c r="G6" s="0">
-        <v>0.4205835034442636</v>
+        <v>0.42330660901653777</v>
       </c>
       <c r="H6" s="0">
         <v>0.75</v>
@@ -674,13 +864,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="0">
-        <v>0.98037421861766749</v>
+        <v>0.9845849463137617</v>
       </c>
       <c r="G14" s="0">
         <v>0</v>
       </c>
       <c r="H14" s="0">
-        <v>0.74499537200879318</v>
+        <v>0.74608591486218567</v>
       </c>
       <c r="I14" s="0"/>
       <c r="J14" s="0">
@@ -707,7 +897,7 @@
         <v>0.59999999999999998</v>
       </c>
       <c r="E15" s="0">
-        <v>0.99725174569692221</v>
+        <v>0.99829545665405295</v>
       </c>
       <c r="F15" s="0">
         <v>0</v>
@@ -716,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="0">
-        <v>0.74931104300947826</v>
+        <v>0.74957313655838465</v>
       </c>
       <c r="I15" s="0"/>
       <c r="J15" s="0">
@@ -890,13 +1080,13 @@
         <v>0</v>
       </c>
       <c r="F20" s="0">
-        <v>0.95250293432896127</v>
+        <v>0.95828872109608543</v>
       </c>
       <c r="G20" s="0">
         <v>0</v>
       </c>
       <c r="H20" s="0">
-        <v>0.73753495276677872</v>
+        <v>0.73911907993526249</v>
       </c>
       <c r="I20" s="0"/>
       <c r="J20" s="0">
@@ -962,13 +1152,13 @@
         <v>0</v>
       </c>
       <c r="F22" s="0">
-        <v>0.88853723600851864</v>
+        <v>0.89583167445557765</v>
       </c>
       <c r="G22" s="0">
         <v>0</v>
       </c>
       <c r="H22" s="0">
-        <v>0.71868212017381472</v>
+        <v>0.72096257493419136</v>
       </c>
       <c r="I22" s="0"/>
       <c r="J22" s="0">

</xml_diff>